<commit_message>
Updated File scanner for Gross profit detials ✅
</commit_message>
<xml_diff>
--- a/Data and Report Management/Data Visualisation/Examplery_data.xlsx
+++ b/Data and Report Management/Data Visualisation/Examplery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Automate\Data and Report Management\Data Visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030D0767-D7AA-4432-A2B9-F6E251D5FFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56625145-6583-406E-A995-E0C73E041BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1808,6 +1808,7 @@
     <xf numFmtId="167" fontId="5" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1826,7 +1827,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2179,8 +2179,8 @@
   <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N22"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2536,7 +2536,7 @@
       <c r="E11" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="180"/>
+      <c r="F11" s="181"/>
       <c r="G11" s="106" t="s">
         <v>6</v>
       </c>
@@ -2546,7 +2546,7 @@
       <c r="I11" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="181"/>
+      <c r="J11" s="182"/>
       <c r="K11" s="114" t="s">
         <v>10</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="M11" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="182"/>
+      <c r="N11" s="183"/>
       <c r="O11" s="130" t="s">
         <v>14</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="Q11" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="R11" s="183"/>
+      <c r="R11" s="184"/>
       <c r="S11"/>
     </row>
     <row r="12" spans="1:19" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2582,7 +2582,7 @@
       <c r="E12" s="163">
         <v>0.75</v>
       </c>
-      <c r="F12" s="180"/>
+      <c r="F12" s="181"/>
       <c r="G12" s="164">
         <v>0.75</v>
       </c>
@@ -2592,7 +2592,7 @@
       <c r="I12" s="164">
         <v>0.75</v>
       </c>
-      <c r="J12" s="181"/>
+      <c r="J12" s="182"/>
       <c r="K12" s="165">
         <v>0.75</v>
       </c>
@@ -2602,7 +2602,7 @@
       <c r="M12" s="165">
         <v>0.75</v>
       </c>
-      <c r="N12" s="182"/>
+      <c r="N12" s="183"/>
       <c r="O12" s="166">
         <v>0.75</v>
       </c>
@@ -2612,7 +2612,7 @@
       <c r="Q12" s="166">
         <v>0.75</v>
       </c>
-      <c r="R12" s="183"/>
+      <c r="R12" s="184"/>
     </row>
     <row r="13" spans="1:19" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="107" t="s">
@@ -2627,7 +2627,7 @@
       <c r="E13" s="163">
         <v>0.25</v>
       </c>
-      <c r="F13" s="180"/>
+      <c r="F13" s="181"/>
       <c r="G13" s="164">
         <v>0.25</v>
       </c>
@@ -2637,7 +2637,7 @@
       <c r="I13" s="164">
         <v>0.25</v>
       </c>
-      <c r="J13" s="181"/>
+      <c r="J13" s="182"/>
       <c r="K13" s="165">
         <v>0.25</v>
       </c>
@@ -2647,7 +2647,7 @@
       <c r="M13" s="165">
         <v>0.25</v>
       </c>
-      <c r="N13" s="182"/>
+      <c r="N13" s="183"/>
       <c r="O13" s="166">
         <v>0.25</v>
       </c>
@@ -2657,7 +2657,7 @@
       <c r="Q13" s="166">
         <v>0.25</v>
       </c>
-      <c r="R13" s="183"/>
+      <c r="R13" s="184"/>
     </row>
     <row r="14" spans="1:19" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="107" t="s">
@@ -2672,7 +2672,7 @@
       <c r="E14" s="110">
         <v>50</v>
       </c>
-      <c r="F14" s="180"/>
+      <c r="F14" s="181"/>
       <c r="G14" s="111">
         <v>50</v>
       </c>
@@ -2682,7 +2682,7 @@
       <c r="I14" s="111">
         <v>50</v>
       </c>
-      <c r="J14" s="181"/>
+      <c r="J14" s="182"/>
       <c r="K14" s="116">
         <v>50</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="M14" s="116">
         <v>50</v>
       </c>
-      <c r="N14" s="182"/>
+      <c r="N14" s="183"/>
       <c r="O14" s="132">
         <v>50</v>
       </c>
@@ -2702,7 +2702,7 @@
       <c r="Q14" s="132">
         <v>50</v>
       </c>
-      <c r="R14" s="183"/>
+      <c r="R14" s="184"/>
     </row>
     <row r="15" spans="1:19" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="107" t="s">
@@ -2717,7 +2717,7 @@
       <c r="E15" s="108">
         <v>7500</v>
       </c>
-      <c r="F15" s="180"/>
+      <c r="F15" s="181"/>
       <c r="G15" s="109">
         <v>7500</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="I15" s="109">
         <v>7500</v>
       </c>
-      <c r="J15" s="181"/>
+      <c r="J15" s="182"/>
       <c r="K15" s="115">
         <v>7500</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="M15" s="115">
         <v>7500</v>
       </c>
-      <c r="N15" s="182"/>
+      <c r="N15" s="183"/>
       <c r="O15" s="131">
         <v>7500</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="Q15" s="131">
         <v>7500</v>
       </c>
-      <c r="R15" s="183"/>
+      <c r="R15" s="184"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B16" s="33"/>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="33" spans="2:19" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O33" s="28">
-        <f t="shared" ref="D33:Q33" si="26">O31-O32</f>
+        <f t="shared" ref="O33:Q33" si="26">O31-O32</f>
         <v>0</v>
       </c>
       <c r="P33" s="27">
@@ -4567,15 +4567,15 @@
       </c>
     </row>
     <row r="137" spans="2:19" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="186"/>
-      <c r="C137" s="186"/>
-      <c r="D137" s="186"/>
-      <c r="E137" s="186"/>
-      <c r="F137" s="186"/>
-      <c r="G137" s="186"/>
-      <c r="H137" s="186"/>
-      <c r="I137" s="186"/>
-      <c r="J137" s="186"/>
+      <c r="B137" s="180"/>
+      <c r="C137" s="180"/>
+      <c r="D137" s="180"/>
+      <c r="E137" s="180"/>
+      <c r="F137" s="180"/>
+      <c r="G137" s="180"/>
+      <c r="H137" s="180"/>
+      <c r="I137" s="180"/>
+      <c r="J137" s="180"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4635,7 +4635,7 @@
       <c r="E2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="184"/>
+      <c r="G2" s="185"/>
     </row>
     <row r="3" spans="1:7" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="51" t="s">
@@ -4653,7 +4653,7 @@
         <f>IFERROR(E29/E54,"")</f>
         <v/>
       </c>
-      <c r="G3" s="184"/>
+      <c r="G3" s="185"/>
     </row>
     <row r="4" spans="1:7" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="51" t="s">
@@ -4671,7 +4671,7 @@
         <f>IFERROR((E29-E26)/(E54-E44),"")</f>
         <v/>
       </c>
-      <c r="G4" s="184"/>
+      <c r="G4" s="185"/>
     </row>
     <row r="5" spans="1:7" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="51" t="s">
@@ -4689,7 +4689,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="184"/>
+      <c r="G5" s="185"/>
     </row>
     <row r="6" spans="1:7" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="51" t="s">
@@ -4707,7 +4707,7 @@
         <f>IFERROR(E63/E40,"")</f>
         <v/>
       </c>
-      <c r="G6" s="184"/>
+      <c r="G6" s="185"/>
     </row>
     <row r="7" spans="1:7" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="51" t="s">
@@ -4725,7 +4725,7 @@
         <f>IFERROR(E63/E72,"")</f>
         <v/>
       </c>
-      <c r="G7" s="184"/>
+      <c r="G7" s="185"/>
     </row>
     <row r="8" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5641,7 +5641,7 @@
         <f>SUM(C17,C26,F14)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="185"/>
+      <c r="E3" s="186"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="39" t="s">
@@ -5651,7 +5651,7 @@
         <f>SUM(C2:C3)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="185"/>
+      <c r="E4" s="186"/>
     </row>
     <row r="5" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="157"/>

</xml_diff>

<commit_message>
Added Monthly Net profit Calculations ✅
</commit_message>
<xml_diff>
--- a/Data and Report Management/Data Visualisation/Examplery_data.xlsx
+++ b/Data and Report Management/Data Visualisation/Examplery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Automate\Data and Report Management\Data Visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56625145-6583-406E-A995-E0C73E041BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107EBA46-6452-4E48-A12F-43C87EDA477D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2180,7 +2180,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updates Sales section for Examplery Data Excel sheet ✅
</commit_message>
<xml_diff>
--- a/Data and Report Management/Data Visualisation/Examplery_data.xlsx
+++ b/Data and Report Management/Data Visualisation/Examplery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Automate\Data and Report Management\Data Visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107EBA46-6452-4E48-A12F-43C87EDA477D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A270B764-3A68-4FE7-951B-172EC3B79152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2179,8 +2179,8 @@
   <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2834,26 +2834,44 @@
       <c r="B19" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
+      <c r="C19" s="101">
+        <v>10000</v>
+      </c>
+      <c r="D19" s="101">
+        <v>15000</v>
+      </c>
+      <c r="E19" s="101">
+        <v>20000</v>
+      </c>
       <c r="F19" s="99">
         <f>SUM(C19:E19)</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
+        <v>45000</v>
+      </c>
+      <c r="G19" s="22">
+        <v>15000</v>
+      </c>
+      <c r="H19" s="22">
+        <v>15000</v>
+      </c>
+      <c r="I19" s="22">
+        <v>30000</v>
+      </c>
       <c r="J19" s="20">
         <f>SUM(G19:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
+        <v>60000</v>
+      </c>
+      <c r="K19" s="18">
+        <v>15000</v>
+      </c>
+      <c r="L19" s="18">
+        <v>30000</v>
+      </c>
+      <c r="M19" s="18">
+        <v>45000</v>
+      </c>
       <c r="N19" s="16">
         <f>SUM(K19:M19)</f>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="O19" s="136"/>
       <c r="P19" s="137"/>
@@ -2864,33 +2882,51 @@
       </c>
       <c r="S19" s="12">
         <f>SUM(F19,J19,N19,R19)</f>
-        <v>0</v>
+        <v>195000</v>
       </c>
     </row>
     <row r="20" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
+      <c r="C20" s="101">
+        <v>3500</v>
+      </c>
+      <c r="D20" s="101">
+        <v>4000</v>
+      </c>
+      <c r="E20" s="101">
+        <v>4500</v>
+      </c>
       <c r="F20" s="99">
         <f>SUM(C20:E20)</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+        <v>12000</v>
+      </c>
+      <c r="G20" s="22">
+        <v>3500</v>
+      </c>
+      <c r="H20" s="8">
+        <v>4000</v>
+      </c>
+      <c r="I20" s="8">
+        <v>5500</v>
+      </c>
       <c r="J20" s="20">
         <f>SUM(G20:I20)</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+        <v>13000</v>
+      </c>
+      <c r="K20" s="18">
+        <v>3500</v>
+      </c>
+      <c r="L20" s="9">
+        <v>5500</v>
+      </c>
+      <c r="M20" s="9">
+        <v>6500</v>
+      </c>
       <c r="N20" s="16">
         <f>SUM(K20:M20)</f>
-        <v>0</v>
+        <v>15500</v>
       </c>
       <c r="O20" s="136"/>
       <c r="P20" s="137"/>
@@ -2901,33 +2937,51 @@
       </c>
       <c r="S20" s="12">
         <f t="shared" ref="S20:S22" si="7">SUM(F20,J20,N20,R20)</f>
-        <v>0</v>
+        <v>40500</v>
       </c>
     </row>
     <row r="21" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="101"/>
+      <c r="C21" s="101">
+        <v>500</v>
+      </c>
+      <c r="D21" s="101">
+        <v>1500</v>
+      </c>
+      <c r="E21" s="101">
+        <v>2000</v>
+      </c>
       <c r="F21" s="99">
         <f>SUM(C21:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+        <v>4000</v>
+      </c>
+      <c r="G21" s="22">
+        <v>2500</v>
+      </c>
+      <c r="H21" s="8">
+        <v>5000</v>
+      </c>
+      <c r="I21" s="8">
+        <v>1200</v>
+      </c>
       <c r="J21" s="20">
         <f>SUM(G21:I21)</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+        <v>8700</v>
+      </c>
+      <c r="K21" s="18">
+        <v>2000</v>
+      </c>
+      <c r="L21" s="9">
+        <v>2500</v>
+      </c>
+      <c r="M21" s="9">
+        <v>25000</v>
+      </c>
       <c r="N21" s="16">
         <f>SUM(K21:M21)</f>
-        <v>0</v>
+        <v>29500</v>
       </c>
       <c r="O21" s="136"/>
       <c r="P21" s="137"/>
@@ -2938,7 +2992,7 @@
       </c>
       <c r="S21" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>42200</v>
       </c>
     </row>
     <row r="22" spans="2:19" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2947,51 +3001,51 @@
       </c>
       <c r="C22" s="25">
         <f>SUM(C19:C21)</f>
-        <v>0</v>
+        <v>14000</v>
       </c>
       <c r="D22" s="25">
         <f t="shared" ref="D22:F22" si="8">SUM(D19:D21)</f>
-        <v>0</v>
+        <v>20500</v>
       </c>
       <c r="E22" s="25">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>26500</v>
       </c>
       <c r="F22" s="29">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>61000</v>
       </c>
       <c r="G22" s="25">
         <f>SUM(G19:G21)</f>
-        <v>0</v>
+        <v>21000</v>
       </c>
       <c r="H22" s="25">
         <f t="shared" ref="H22" si="9">SUM(H19:H21)</f>
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="I22" s="25">
         <f t="shared" ref="I22" si="10">SUM(I19:I21)</f>
-        <v>0</v>
+        <v>36700</v>
       </c>
       <c r="J22" s="31">
         <f t="shared" ref="J22" si="11">SUM(J19:J21)</f>
-        <v>0</v>
+        <v>81700</v>
       </c>
       <c r="K22" s="25">
         <f>SUM(K19:K21)</f>
-        <v>0</v>
+        <v>20500</v>
       </c>
       <c r="L22" s="25">
         <f t="shared" ref="L22" si="12">SUM(L19:L21)</f>
-        <v>0</v>
+        <v>38000</v>
       </c>
       <c r="M22" s="25">
         <f t="shared" ref="M22" si="13">SUM(M19:M21)</f>
-        <v>0</v>
+        <v>76500</v>
       </c>
       <c r="N22" s="31">
         <f t="shared" ref="N22" si="14">SUM(N19:N21)</f>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="O22" s="25">
         <f>SUM(O19:O21)</f>
@@ -3011,7 +3065,7 @@
       </c>
       <c r="S22" s="32">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>277700</v>
       </c>
     </row>
     <row r="23" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added monthly sales value ✅
</commit_message>
<xml_diff>
--- a/Data and Report Management/Data Visualisation/Examplery_data.xlsx
+++ b/Data and Report Management/Data Visualisation/Examplery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Automate\Data and Report Management\Data Visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A270B764-3A68-4FE7-951B-172EC3B79152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92148B51-1228-46F5-8916-055FADF9A9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2180,7 +2180,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Monthly Commissions values ✅
</commit_message>
<xml_diff>
--- a/Data and Report Management/Data Visualisation/Examplery_data.xlsx
+++ b/Data and Report Management/Data Visualisation/Examplery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Automate\Data and Report Management\Data Visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92148B51-1228-46F5-8916-055FADF9A9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0623143D-127C-41F6-9D40-B15D239F6742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2180,7 +2180,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Total Sales values ✅
</commit_message>
<xml_diff>
--- a/Data and Report Management/Data Visualisation/Examplery_data.xlsx
+++ b/Data and Report Management/Data Visualisation/Examplery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Automate\Data and Report Management\Data Visualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0623143D-127C-41F6-9D40-B15D239F6742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CE1459-8511-496A-9CA9-67D7CC73EC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2180,7 +2180,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2873,16 +2873,22 @@
         <f>SUM(K19:M19)</f>
         <v>90000</v>
       </c>
-      <c r="O19" s="136"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="137"/>
+      <c r="O19" s="136">
+        <v>15000</v>
+      </c>
+      <c r="P19" s="137">
+        <v>30000</v>
+      </c>
+      <c r="Q19" s="137">
+        <v>45000</v>
+      </c>
       <c r="R19" s="148">
         <f>SUM(O19:Q19)</f>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S19" s="12">
         <f>SUM(F19,J19,N19,R19)</f>
-        <v>195000</v>
+        <v>285000</v>
       </c>
     </row>
     <row r="20" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2928,16 +2934,22 @@
         <f>SUM(K20:M20)</f>
         <v>15500</v>
       </c>
-      <c r="O20" s="136"/>
-      <c r="P20" s="137"/>
-      <c r="Q20" s="137"/>
+      <c r="O20" s="136">
+        <v>3500</v>
+      </c>
+      <c r="P20" s="137">
+        <v>5500</v>
+      </c>
+      <c r="Q20" s="137">
+        <v>6500</v>
+      </c>
       <c r="R20" s="148">
         <f>SUM(O20:Q20)</f>
-        <v>0</v>
+        <v>15500</v>
       </c>
       <c r="S20" s="12">
         <f t="shared" ref="S20:S22" si="7">SUM(F20,J20,N20,R20)</f>
-        <v>40500</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="21" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2983,16 +2995,22 @@
         <f>SUM(K21:M21)</f>
         <v>29500</v>
       </c>
-      <c r="O21" s="136"/>
-      <c r="P21" s="137"/>
-      <c r="Q21" s="137"/>
+      <c r="O21" s="136">
+        <v>2000</v>
+      </c>
+      <c r="P21" s="137">
+        <v>2500</v>
+      </c>
+      <c r="Q21" s="137">
+        <v>25000</v>
+      </c>
       <c r="R21" s="148">
         <f>SUM(O21:Q21)</f>
-        <v>0</v>
+        <v>29500</v>
       </c>
       <c r="S21" s="12">
         <f t="shared" si="7"/>
-        <v>42200</v>
+        <v>71700</v>
       </c>
     </row>
     <row r="22" spans="2:19" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3049,23 +3067,23 @@
       </c>
       <c r="O22" s="25">
         <f>SUM(O19:O21)</f>
-        <v>0</v>
+        <v>20500</v>
       </c>
       <c r="P22" s="25">
         <f t="shared" ref="P22" si="15">SUM(P19:P21)</f>
-        <v>0</v>
+        <v>38000</v>
       </c>
       <c r="Q22" s="25">
         <f t="shared" ref="Q22" si="16">SUM(Q19:Q21)</f>
-        <v>0</v>
+        <v>76500</v>
       </c>
       <c r="R22" s="31">
         <f t="shared" ref="R22" si="17">SUM(R19:R21)</f>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="S22" s="32">
         <f t="shared" si="7"/>
-        <v>277700</v>
+        <v>412700</v>
       </c>
     </row>
     <row r="23" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -3126,23 +3144,23 @@
     <row r="27" spans="2:19" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O27" s="28">
         <f>O22-O26</f>
-        <v>0</v>
+        <v>20500</v>
       </c>
       <c r="P27" s="27">
         <f t="shared" ref="P27" si="21">P22-P26</f>
-        <v>0</v>
+        <v>38000</v>
       </c>
       <c r="Q27" s="27">
         <f t="shared" ref="Q27" si="22">Q22-Q26</f>
-        <v>0</v>
+        <v>76500</v>
       </c>
       <c r="R27" s="26">
         <f t="shared" ref="R27" si="23">R22-R26</f>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="S27" s="32">
         <f>SUM(F27,J27,N27,R27)</f>
-        <v>0</v>
+        <v>135000</v>
       </c>
     </row>
     <row r="28" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -3238,23 +3256,23 @@
     <row r="34" spans="2:19" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O34" s="133">
         <f>O27-O33</f>
-        <v>0</v>
+        <v>20500</v>
       </c>
       <c r="P34" s="134">
         <f t="shared" ref="P34" si="27">P27-P33</f>
-        <v>0</v>
+        <v>38000</v>
       </c>
       <c r="Q34" s="134">
         <f t="shared" ref="Q34" si="28">Q27-Q33</f>
-        <v>0</v>
+        <v>76500</v>
       </c>
       <c r="R34" s="149">
         <f>SUM(O34:Q34)</f>
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="S34" s="152">
         <f>SUM(F34,J34,N34,R34)</f>
-        <v>0</v>
+        <v>135000</v>
       </c>
     </row>
     <row r="36" spans="2:19" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>